<commit_message>
*delete button und likes
</commit_message>
<xml_diff>
--- a/190503StartseitenkonzeptB.xlsx
+++ b/190503StartseitenkonzeptB.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lc_admin.planks/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lc_admin.planks/Documents/ttt/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090351AE-1072-6545-BB17-DB0076079934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="50780" windowHeight="26720"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="117">
   <si>
     <t>Homepage</t>
   </si>
@@ -454,12 +455,15 @@
   <si>
     <t>Name??</t>
   </si>
+  <si>
+    <t>https://vegibit.com/how-to-delete-an-item-from-an-array-in-react/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +543,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -1248,10 +1260,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1629,6 +1642,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1638,12 +1699,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1665,51 +1720,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1744,7 +1759,7 @@
         <xdr:cNvPr id="1025" name="AutoShape 1" descr="(Fehler)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1792,7 +1807,7 @@
         <xdr:cNvPr id="1026" name="AutoShape 2" descr="(Fehler)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1840,7 +1855,7 @@
         <xdr:cNvPr id="1027" name="AutoShape 3" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1888,7 +1903,7 @@
         <xdr:cNvPr id="1028" name="AutoShape 4" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1936,7 +1951,7 @@
         <xdr:cNvPr id="1029" name="AutoShape 5" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1984,7 +1999,7 @@
         <xdr:cNvPr id="1030" name="AutoShape 6" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2027,7 +2042,7 @@
         <xdr:cNvPr id="8" name="AutoShape 2" descr="(Fehler)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2070,7 +2085,7 @@
         <xdr:cNvPr id="9" name="AutoShape 3" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2113,7 +2128,7 @@
         <xdr:cNvPr id="10" name="AutoShape 4" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2156,7 +2171,7 @@
         <xdr:cNvPr id="11" name="AutoShape 5" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2199,7 +2214,7 @@
         <xdr:cNvPr id="12" name="AutoShape 2" descr="(Fehler)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2242,7 +2257,7 @@
         <xdr:cNvPr id="13" name="AutoShape 3" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2285,7 +2300,7 @@
         <xdr:cNvPr id="14" name="AutoShape 4" descr="(Haken)">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2604,14 +2619,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H152"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="C147" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
@@ -2621,7 +2636,7 @@
     <col min="7" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="34">
       <c r="A1" s="23" t="s">
         <v>32</v>
       </c>
@@ -2642,7 +2657,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="20" thickBot="1">
       <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
@@ -2653,7 +2668,7 @@
       <c r="F2" s="30"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="20" thickBot="1">
       <c r="A3" s="26" t="s">
         <v>3</v>
       </c>
@@ -2664,7 +2679,7 @@
       <c r="F3" s="31"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="21" thickTop="1" thickBot="1">
       <c r="A4" s="27" t="s">
         <v>30</v>
       </c>
@@ -2684,8 +2699,8 @@
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
     </row>
-    <row r="5" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="140" t="s">
+    <row r="5" spans="1:8" ht="38.25" customHeight="1">
+      <c r="A5" s="130" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2706,8 +2721,8 @@
       <c r="G5" s="19"/>
       <c r="H5" s="18"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="141"/>
+    <row r="6" spans="1:8" ht="18">
+      <c r="A6" s="131"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2726,8 +2741,8 @@
       <c r="G6" s="20"/>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="141"/>
+    <row r="7" spans="1:8" ht="52.5" customHeight="1">
+      <c r="A7" s="131"/>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
@@ -2748,8 +2763,8 @@
       </c>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="141"/>
+    <row r="8" spans="1:8" ht="18">
+      <c r="A8" s="131"/>
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
@@ -2768,8 +2783,8 @@
       <c r="G8" s="20"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="141"/>
+    <row r="9" spans="1:8" ht="18">
+      <c r="A9" s="131"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -2788,8 +2803,8 @@
       <c r="G9" s="20"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="141"/>
+    <row r="10" spans="1:8" ht="18">
+      <c r="A10" s="131"/>
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
@@ -2808,8 +2823,8 @@
       <c r="G10" s="21"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="142"/>
+    <row r="11" spans="1:8" ht="19" thickBot="1">
+      <c r="A11" s="132"/>
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -2828,8 +2843,8 @@
       <c r="G11" s="22"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="140" t="s">
+    <row r="12" spans="1:8" ht="32">
+      <c r="A12" s="130" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -2849,8 +2864,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="141"/>
+    <row r="13" spans="1:8" ht="18">
+      <c r="A13" s="131"/>
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
@@ -2866,8 +2881,8 @@
       <c r="F13" s="49"/>
       <c r="G13" s="50"/>
     </row>
-    <row r="14" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="141"/>
+    <row r="14" spans="1:8" ht="31.5" customHeight="1">
+      <c r="A14" s="131"/>
       <c r="B14" s="8" t="s">
         <v>6</v>
       </c>
@@ -2883,8 +2898,8 @@
       <c r="F14" s="49"/>
       <c r="G14" s="50"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="141"/>
+    <row r="15" spans="1:8" ht="18">
+      <c r="A15" s="131"/>
       <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2901,8 +2916,8 @@
       <c r="G15" s="52"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="141"/>
+    <row r="16" spans="1:8" ht="18">
+      <c r="A16" s="131"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2918,8 +2933,8 @@
       <c r="F16" s="49"/>
       <c r="G16" s="50"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="141"/>
+    <row r="17" spans="1:8" ht="18">
+      <c r="A17" s="131"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -2936,8 +2951,8 @@
       <c r="G17" s="52"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="142"/>
+    <row r="18" spans="1:8" ht="19" thickBot="1">
+      <c r="A18" s="132"/>
       <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
@@ -2954,7 +2969,7 @@
       <c r="G18" s="60"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="1:8" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="58" thickBot="1">
       <c r="A19" s="61" t="s">
         <v>110</v>
       </c>
@@ -2974,8 +2989,8 @@
       </c>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="140" t="s">
+    <row r="20" spans="1:8" ht="32">
+      <c r="A20" s="130" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -2990,8 +3005,8 @@
       <c r="G20" s="69"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="143"/>
+    <row r="21" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A21" s="133"/>
       <c r="B21" s="8" t="s">
         <v>5</v>
       </c>
@@ -3003,8 +3018,8 @@
       <c r="F21" s="49"/>
       <c r="G21" s="50"/>
     </row>
-    <row r="22" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="143"/>
+    <row r="22" spans="1:8" ht="35.25" customHeight="1">
+      <c r="A22" s="133"/>
       <c r="B22" s="8" t="s">
         <v>6</v>
       </c>
@@ -3016,8 +3031,8 @@
       <c r="F22" s="49"/>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="143"/>
+    <row r="23" spans="1:8" ht="32">
+      <c r="A23" s="133"/>
       <c r="B23" s="8" t="s">
         <v>7</v>
       </c>
@@ -3029,8 +3044,8 @@
       <c r="F23" s="49"/>
       <c r="G23" s="50"/>
     </row>
-    <row r="24" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="143"/>
+    <row r="24" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A24" s="133"/>
       <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
@@ -3042,8 +3057,8 @@
       <c r="F24" s="49"/>
       <c r="G24" s="50"/>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="143"/>
+    <row r="25" spans="1:8" ht="32">
+      <c r="A25" s="133"/>
       <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
@@ -3055,8 +3070,8 @@
       <c r="F25" s="49"/>
       <c r="G25" s="50"/>
     </row>
-    <row r="26" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="144"/>
+    <row r="26" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A26" s="134"/>
       <c r="B26" s="12" t="s">
         <v>10</v>
       </c>
@@ -3068,8 +3083,8 @@
       <c r="F26" s="114"/>
       <c r="G26" s="77"/>
     </row>
-    <row r="27" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="146" t="s">
+    <row r="27" spans="1:8" ht="36.75" customHeight="1">
+      <c r="A27" s="136" t="s">
         <v>85</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -3090,8 +3105,8 @@
       </c>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="147"/>
+    <row r="28" spans="1:8" ht="18">
+      <c r="A28" s="137"/>
       <c r="B28" s="8" t="s">
         <v>5</v>
       </c>
@@ -3107,8 +3122,8 @@
       </c>
       <c r="G28" s="50"/>
     </row>
-    <row r="29" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="147"/>
+    <row r="29" spans="1:8" ht="50.25" customHeight="1">
+      <c r="A29" s="137"/>
       <c r="B29" s="8" t="s">
         <v>6</v>
       </c>
@@ -3124,8 +3139,8 @@
       </c>
       <c r="G29" s="50"/>
     </row>
-    <row r="30" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="147"/>
+    <row r="30" spans="1:8" ht="22.5" customHeight="1">
+      <c r="A30" s="137"/>
       <c r="B30" s="8" t="s">
         <v>7</v>
       </c>
@@ -3141,8 +3156,8 @@
       </c>
       <c r="G30" s="50"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="147"/>
+    <row r="31" spans="1:8" ht="18">
+      <c r="A31" s="137"/>
       <c r="B31" s="8" t="s">
         <v>8</v>
       </c>
@@ -3158,8 +3173,8 @@
       </c>
       <c r="G31" s="50"/>
     </row>
-    <row r="32" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="147"/>
+    <row r="32" spans="1:8" ht="82.5" customHeight="1">
+      <c r="A32" s="137"/>
       <c r="B32" s="8" t="s">
         <v>9</v>
       </c>
@@ -3175,8 +3190,8 @@
       </c>
       <c r="G32" s="50"/>
     </row>
-    <row r="33" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="147"/>
+    <row r="33" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
+      <c r="A33" s="137"/>
       <c r="B33" s="12" t="s">
         <v>10</v>
       </c>
@@ -3192,8 +3207,8 @@
       </c>
       <c r="G33" s="77"/>
     </row>
-    <row r="34" spans="1:8" ht="31" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="146" t="s">
+    <row r="34" spans="1:8" ht="33" thickTop="1">
+      <c r="A34" s="136" t="s">
         <v>100</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -3208,8 +3223,8 @@
       <c r="G34" s="47"/>
       <c r="H34" s="18"/>
     </row>
-    <row r="35" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="151"/>
+    <row r="35" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A35" s="141"/>
       <c r="B35" s="8" t="s">
         <v>5</v>
       </c>
@@ -3221,8 +3236,8 @@
       </c>
       <c r="G35" s="50"/>
     </row>
-    <row r="36" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="151"/>
+    <row r="36" spans="1:8" ht="35.25" customHeight="1">
+      <c r="A36" s="141"/>
       <c r="B36" s="8" t="s">
         <v>6</v>
       </c>
@@ -3234,8 +3249,8 @@
       </c>
       <c r="G36" s="50"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="151"/>
+    <row r="37" spans="1:8" ht="18">
+      <c r="A37" s="141"/>
       <c r="B37" s="8" t="s">
         <v>7</v>
       </c>
@@ -3247,8 +3262,8 @@
       </c>
       <c r="G37" s="50"/>
     </row>
-    <row r="38" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="151"/>
+    <row r="38" spans="1:8" ht="16.5" customHeight="1">
+      <c r="A38" s="141"/>
       <c r="B38" s="8" t="s">
         <v>8</v>
       </c>
@@ -3260,8 +3275,8 @@
       </c>
       <c r="G38" s="50"/>
     </row>
-    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A39" s="151"/>
+    <row r="39" spans="1:8" ht="64">
+      <c r="A39" s="141"/>
       <c r="B39" s="8" t="s">
         <v>9</v>
       </c>
@@ -3273,8 +3288,8 @@
       </c>
       <c r="G39" s="50"/>
     </row>
-    <row r="40" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="152"/>
+    <row r="40" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A40" s="142"/>
       <c r="B40" s="12" t="s">
         <v>10</v>
       </c>
@@ -3286,8 +3301,8 @@
       </c>
       <c r="G40" s="77"/>
     </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" s="146" t="s">
+    <row r="41" spans="1:8" ht="32">
+      <c r="A41" s="136" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -3304,8 +3319,8 @@
       <c r="G41" s="47"/>
       <c r="H41" s="18"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="147"/>
+    <row r="42" spans="1:8" ht="18">
+      <c r="A42" s="137"/>
       <c r="B42" s="8" t="s">
         <v>5</v>
       </c>
@@ -3319,8 +3334,8 @@
       </c>
       <c r="G42" s="50"/>
     </row>
-    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="147"/>
+    <row r="43" spans="1:8" ht="32">
+      <c r="A43" s="137"/>
       <c r="B43" s="8" t="s">
         <v>6</v>
       </c>
@@ -3334,8 +3349,8 @@
       </c>
       <c r="G43" s="50"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="147"/>
+    <row r="44" spans="1:8" ht="18">
+      <c r="A44" s="137"/>
       <c r="B44" s="8" t="s">
         <v>7</v>
       </c>
@@ -3349,8 +3364,8 @@
       </c>
       <c r="G44" s="50"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="147"/>
+    <row r="45" spans="1:8" ht="18">
+      <c r="A45" s="137"/>
       <c r="B45" s="8" t="s">
         <v>8</v>
       </c>
@@ -3364,8 +3379,8 @@
       </c>
       <c r="G45" s="50"/>
     </row>
-    <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A46" s="147"/>
+    <row r="46" spans="1:8" ht="48">
+      <c r="A46" s="137"/>
       <c r="B46" s="8" t="s">
         <v>9</v>
       </c>
@@ -3379,8 +3394,8 @@
       </c>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="147"/>
+    <row r="47" spans="1:8" ht="19" thickBot="1">
+      <c r="A47" s="137"/>
       <c r="B47" s="12" t="s">
         <v>10</v>
       </c>
@@ -3394,8 +3409,8 @@
       </c>
       <c r="G47" s="77"/>
     </row>
-    <row r="48" spans="1:8" ht="31" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="146" t="s">
+    <row r="48" spans="1:8" ht="33" thickTop="1">
+      <c r="A48" s="136" t="s">
         <v>114</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -3416,8 +3431,8 @@
       </c>
       <c r="H48" s="18"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="147"/>
+    <row r="49" spans="1:7" ht="18">
+      <c r="A49" s="137"/>
       <c r="B49" s="8" t="s">
         <v>5</v>
       </c>
@@ -3433,8 +3448,8 @@
       </c>
       <c r="G49" s="50"/>
     </row>
-    <row r="50" spans="1:7" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="147"/>
+    <row r="50" spans="1:7" ht="93.75" customHeight="1">
+      <c r="A50" s="137"/>
       <c r="B50" s="8" t="s">
         <v>6</v>
       </c>
@@ -3450,8 +3465,8 @@
       </c>
       <c r="G50" s="50"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="147"/>
+    <row r="51" spans="1:7" ht="18">
+      <c r="A51" s="137"/>
       <c r="B51" s="8" t="s">
         <v>7</v>
       </c>
@@ -3467,8 +3482,8 @@
       </c>
       <c r="G51" s="50"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="147"/>
+    <row r="52" spans="1:7" ht="18">
+      <c r="A52" s="137"/>
       <c r="B52" s="8" t="s">
         <v>8</v>
       </c>
@@ -3484,8 +3499,8 @@
       </c>
       <c r="G52" s="50"/>
     </row>
-    <row r="53" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="147"/>
+    <row r="53" spans="1:7" ht="65.25" customHeight="1">
+      <c r="A53" s="137"/>
       <c r="B53" s="8" t="s">
         <v>9</v>
       </c>
@@ -3501,8 +3516,8 @@
       </c>
       <c r="G53" s="50"/>
     </row>
-    <row r="54" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="147"/>
+    <row r="54" spans="1:7" ht="19" thickBot="1">
+      <c r="A54" s="137"/>
       <c r="B54" s="12" t="s">
         <v>10</v>
       </c>
@@ -3518,8 +3533,8 @@
       </c>
       <c r="G54" s="77"/>
     </row>
-    <row r="55" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="145" t="s">
+    <row r="55" spans="1:7" ht="19" thickTop="1">
+      <c r="A55" s="135" t="s">
         <v>18</v>
       </c>
       <c r="B55" s="13" t="s">
@@ -3533,8 +3548,8 @@
       <c r="F55" s="80"/>
       <c r="G55" s="81"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="131"/>
+    <row r="56" spans="1:7" ht="18">
+      <c r="A56" s="128"/>
       <c r="B56" s="8" t="s">
         <v>5</v>
       </c>
@@ -3544,8 +3559,8 @@
       <c r="F56" s="49"/>
       <c r="G56" s="82"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="131"/>
+    <row r="57" spans="1:7" ht="18">
+      <c r="A57" s="128"/>
       <c r="B57" s="8" t="s">
         <v>6</v>
       </c>
@@ -3555,8 +3570,8 @@
       <c r="F57" s="49"/>
       <c r="G57" s="82"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="131"/>
+    <row r="58" spans="1:7" ht="18">
+      <c r="A58" s="128"/>
       <c r="B58" s="8" t="s">
         <v>7</v>
       </c>
@@ -3566,8 +3581,8 @@
       <c r="F58" s="49"/>
       <c r="G58" s="82"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="131"/>
+    <row r="59" spans="1:7" ht="18">
+      <c r="A59" s="128"/>
       <c r="B59" s="8" t="s">
         <v>8</v>
       </c>
@@ -3577,8 +3592,8 @@
       <c r="F59" s="49"/>
       <c r="G59" s="82"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="131"/>
+    <row r="60" spans="1:7" ht="18">
+      <c r="A60" s="128"/>
       <c r="B60" s="8" t="s">
         <v>9</v>
       </c>
@@ -3588,8 +3603,8 @@
       <c r="F60" s="49"/>
       <c r="G60" s="82"/>
     </row>
-    <row r="61" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="139"/>
+    <row r="61" spans="1:7" ht="19" thickBot="1">
+      <c r="A61" s="129"/>
       <c r="B61" s="11" t="s">
         <v>10</v>
       </c>
@@ -3599,8 +3614,8 @@
       <c r="F61" s="59"/>
       <c r="G61" s="84"/>
     </row>
-    <row r="62" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A62" s="130" t="s">
+    <row r="62" spans="1:7" ht="32">
+      <c r="A62" s="127" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -3618,8 +3633,8 @@
       <c r="F62" s="46"/>
       <c r="G62" s="85"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="131"/>
+    <row r="63" spans="1:7" ht="18">
+      <c r="A63" s="128"/>
       <c r="B63" s="8" t="s">
         <v>5</v>
       </c>
@@ -3629,8 +3644,8 @@
       <c r="F63" s="49"/>
       <c r="G63" s="82"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="131"/>
+    <row r="64" spans="1:7" ht="18">
+      <c r="A64" s="128"/>
       <c r="B64" s="8" t="s">
         <v>6</v>
       </c>
@@ -3646,8 +3661,8 @@
       <c r="F64" s="49"/>
       <c r="G64" s="82"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="131"/>
+    <row r="65" spans="1:7" ht="18">
+      <c r="A65" s="128"/>
       <c r="B65" s="8" t="s">
         <v>7</v>
       </c>
@@ -3657,8 +3672,8 @@
       <c r="F65" s="49"/>
       <c r="G65" s="82"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="131"/>
+    <row r="66" spans="1:7" ht="18">
+      <c r="A66" s="128"/>
       <c r="B66" s="8" t="s">
         <v>8</v>
       </c>
@@ -3668,8 +3683,8 @@
       <c r="F66" s="49"/>
       <c r="G66" s="82"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="131"/>
+    <row r="67" spans="1:7" ht="18">
+      <c r="A67" s="128"/>
       <c r="B67" s="8" t="s">
         <v>9</v>
       </c>
@@ -3679,8 +3694,8 @@
       <c r="F67" s="49"/>
       <c r="G67" s="82"/>
     </row>
-    <row r="68" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="139"/>
+    <row r="68" spans="1:7" ht="19" thickBot="1">
+      <c r="A68" s="129"/>
       <c r="B68" s="11" t="s">
         <v>10</v>
       </c>
@@ -3690,8 +3705,8 @@
       <c r="F68" s="59"/>
       <c r="G68" s="84"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="130" t="s">
+    <row r="69" spans="1:7" ht="18">
+      <c r="A69" s="127" t="s">
         <v>20</v>
       </c>
       <c r="B69" s="6" t="s">
@@ -3707,8 +3722,8 @@
       <c r="F69" s="46"/>
       <c r="G69" s="85"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="131"/>
+    <row r="70" spans="1:7" ht="18">
+      <c r="A70" s="128"/>
       <c r="B70" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,8 +3733,8 @@
       <c r="F70" s="49"/>
       <c r="G70" s="82"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="131"/>
+    <row r="71" spans="1:7" ht="18">
+      <c r="A71" s="128"/>
       <c r="B71" s="8" t="s">
         <v>6</v>
       </c>
@@ -3731,8 +3746,8 @@
       <c r="F71" s="49"/>
       <c r="G71" s="82"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="131"/>
+    <row r="72" spans="1:7" ht="18">
+      <c r="A72" s="128"/>
       <c r="B72" s="8" t="s">
         <v>7</v>
       </c>
@@ -3742,8 +3757,8 @@
       <c r="F72" s="49"/>
       <c r="G72" s="82"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="131"/>
+    <row r="73" spans="1:7" ht="18">
+      <c r="A73" s="128"/>
       <c r="B73" s="8" t="s">
         <v>8</v>
       </c>
@@ -3753,8 +3768,8 @@
       <c r="F73" s="49"/>
       <c r="G73" s="82"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="131"/>
+    <row r="74" spans="1:7" ht="18">
+      <c r="A74" s="128"/>
       <c r="B74" s="8" t="s">
         <v>9</v>
       </c>
@@ -3764,8 +3779,8 @@
       <c r="F74" s="49"/>
       <c r="G74" s="82"/>
     </row>
-    <row r="75" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="139"/>
+    <row r="75" spans="1:7" ht="19" thickBot="1">
+      <c r="A75" s="129"/>
       <c r="B75" s="11" t="s">
         <v>10</v>
       </c>
@@ -3775,8 +3790,8 @@
       <c r="F75" s="59"/>
       <c r="G75" s="84"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="130" t="s">
+    <row r="76" spans="1:7" ht="18">
+      <c r="A76" s="127" t="s">
         <v>21</v>
       </c>
       <c r="B76" s="6" t="s">
@@ -3790,8 +3805,8 @@
       <c r="F76" s="46"/>
       <c r="G76" s="85"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="131"/>
+    <row r="77" spans="1:7" ht="18">
+      <c r="A77" s="128"/>
       <c r="B77" s="8" t="s">
         <v>5</v>
       </c>
@@ -3801,8 +3816,8 @@
       <c r="F77" s="49"/>
       <c r="G77" s="82"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="131"/>
+    <row r="78" spans="1:7" ht="18">
+      <c r="A78" s="128"/>
       <c r="B78" s="8" t="s">
         <v>6</v>
       </c>
@@ -3812,8 +3827,8 @@
       <c r="F78" s="49"/>
       <c r="G78" s="82"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="131"/>
+    <row r="79" spans="1:7" ht="18">
+      <c r="A79" s="128"/>
       <c r="B79" s="8" t="s">
         <v>7</v>
       </c>
@@ -3823,8 +3838,8 @@
       <c r="F79" s="49"/>
       <c r="G79" s="82"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="131"/>
+    <row r="80" spans="1:7" ht="18">
+      <c r="A80" s="128"/>
       <c r="B80" s="8" t="s">
         <v>8</v>
       </c>
@@ -3834,8 +3849,8 @@
       <c r="F80" s="49"/>
       <c r="G80" s="82"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="131"/>
+    <row r="81" spans="1:7" ht="18">
+      <c r="A81" s="128"/>
       <c r="B81" s="8" t="s">
         <v>9</v>
       </c>
@@ -3845,8 +3860,8 @@
       <c r="F81" s="49"/>
       <c r="G81" s="82"/>
     </row>
-    <row r="82" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="139"/>
+    <row r="82" spans="1:7" ht="19" thickBot="1">
+      <c r="A82" s="129"/>
       <c r="B82" s="11" t="s">
         <v>10</v>
       </c>
@@ -3856,8 +3871,8 @@
       <c r="F82" s="59"/>
       <c r="G82" s="84"/>
     </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A83" s="130" t="s">
+    <row r="83" spans="1:7" ht="64">
+      <c r="A83" s="127" t="s">
         <v>22</v>
       </c>
       <c r="B83" s="6" t="s">
@@ -3877,8 +3892,8 @@
       </c>
       <c r="G83" s="85"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="131"/>
+    <row r="84" spans="1:7" ht="18">
+      <c r="A84" s="128"/>
       <c r="B84" s="8" t="s">
         <v>5</v>
       </c>
@@ -3896,8 +3911,8 @@
       </c>
       <c r="G84" s="82"/>
     </row>
-    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A85" s="131"/>
+    <row r="85" spans="1:7" ht="48">
+      <c r="A85" s="128"/>
       <c r="B85" s="8" t="s">
         <v>6</v>
       </c>
@@ -3915,8 +3930,8 @@
       </c>
       <c r="G85" s="82"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="131"/>
+    <row r="86" spans="1:7" ht="18">
+      <c r="A86" s="128"/>
       <c r="B86" s="8" t="s">
         <v>7</v>
       </c>
@@ -3934,8 +3949,8 @@
       </c>
       <c r="G86" s="82"/>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A87" s="131"/>
+    <row r="87" spans="1:7" ht="32">
+      <c r="A87" s="128"/>
       <c r="B87" s="8" t="s">
         <v>8</v>
       </c>
@@ -3953,8 +3968,8 @@
       </c>
       <c r="G87" s="82"/>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A88" s="131"/>
+    <row r="88" spans="1:7" ht="32">
+      <c r="A88" s="128"/>
       <c r="B88" s="8" t="s">
         <v>9</v>
       </c>
@@ -3972,8 +3987,8 @@
       </c>
       <c r="G88" s="82"/>
     </row>
-    <row r="89" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="139"/>
+    <row r="89" spans="1:7" ht="19" thickBot="1">
+      <c r="A89" s="129"/>
       <c r="B89" s="11" t="s">
         <v>10</v>
       </c>
@@ -3991,8 +4006,8 @@
       </c>
       <c r="G89" s="84"/>
     </row>
-    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A90" s="148" t="s">
+    <row r="90" spans="1:7" ht="48">
+      <c r="A90" s="138" t="s">
         <v>86</v>
       </c>
       <c r="B90" s="6" t="s">
@@ -4010,8 +4025,8 @@
       </c>
       <c r="G90" s="85"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="149"/>
+    <row r="91" spans="1:7" ht="18">
+      <c r="A91" s="139"/>
       <c r="B91" s="8" t="s">
         <v>5</v>
       </c>
@@ -4027,8 +4042,8 @@
       </c>
       <c r="G91" s="82"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="149"/>
+    <row r="92" spans="1:7" ht="18">
+      <c r="A92" s="139"/>
       <c r="B92" s="8" t="s">
         <v>6</v>
       </c>
@@ -4044,8 +4059,8 @@
       </c>
       <c r="G92" s="82"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="149"/>
+    <row r="93" spans="1:7" ht="18">
+      <c r="A93" s="139"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
       </c>
@@ -4061,8 +4076,8 @@
       </c>
       <c r="G93" s="82"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="149"/>
+    <row r="94" spans="1:7" ht="18">
+      <c r="A94" s="139"/>
       <c r="B94" s="8" t="s">
         <v>8</v>
       </c>
@@ -4078,8 +4093,8 @@
       </c>
       <c r="G94" s="82"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="149"/>
+    <row r="95" spans="1:7" ht="18">
+      <c r="A95" s="139"/>
       <c r="B95" s="8" t="s">
         <v>9</v>
       </c>
@@ -4095,8 +4110,8 @@
       </c>
       <c r="G95" s="82"/>
     </row>
-    <row r="96" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="150"/>
+    <row r="96" spans="1:7" ht="19" thickBot="1">
+      <c r="A96" s="140"/>
       <c r="B96" s="11" t="s">
         <v>10</v>
       </c>
@@ -4112,8 +4127,8 @@
       </c>
       <c r="G96" s="84"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="130" t="s">
+    <row r="97" spans="1:7" ht="32">
+      <c r="A97" s="127" t="s">
         <v>23</v>
       </c>
       <c r="B97" s="6" t="s">
@@ -4127,8 +4142,8 @@
       <c r="F97" s="46"/>
       <c r="G97" s="85"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="131"/>
+    <row r="98" spans="1:7" ht="18">
+      <c r="A98" s="128"/>
       <c r="B98" s="8" t="s">
         <v>5</v>
       </c>
@@ -4140,8 +4155,8 @@
       <c r="F98" s="49"/>
       <c r="G98" s="82"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="131"/>
+    <row r="99" spans="1:7" ht="18">
+      <c r="A99" s="128"/>
       <c r="B99" s="8" t="s">
         <v>6</v>
       </c>
@@ -4153,8 +4168,8 @@
       <c r="F99" s="49"/>
       <c r="G99" s="82"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="131"/>
+    <row r="100" spans="1:7" ht="18">
+      <c r="A100" s="128"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
       </c>
@@ -4166,8 +4181,8 @@
       <c r="F100" s="49"/>
       <c r="G100" s="82"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="131"/>
+    <row r="101" spans="1:7" ht="18">
+      <c r="A101" s="128"/>
       <c r="B101" s="8" t="s">
         <v>8</v>
       </c>
@@ -4179,8 +4194,8 @@
       <c r="F101" s="49"/>
       <c r="G101" s="82"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="131"/>
+    <row r="102" spans="1:7" ht="18">
+      <c r="A102" s="128"/>
       <c r="B102" s="8" t="s">
         <v>9</v>
       </c>
@@ -4192,8 +4207,8 @@
       <c r="F102" s="49"/>
       <c r="G102" s="82"/>
     </row>
-    <row r="103" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="139"/>
+    <row r="103" spans="1:7" ht="19" thickBot="1">
+      <c r="A103" s="129"/>
       <c r="B103" s="11" t="s">
         <v>10</v>
       </c>
@@ -4205,8 +4220,8 @@
       <c r="F103" s="59"/>
       <c r="G103" s="84"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" s="130" t="s">
+    <row r="104" spans="1:7" ht="18">
+      <c r="A104" s="127" t="s">
         <v>24</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -4226,8 +4241,8 @@
       </c>
       <c r="G104" s="85"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="131"/>
+    <row r="105" spans="1:7" ht="18">
+      <c r="A105" s="128"/>
       <c r="B105" s="8" t="s">
         <v>5</v>
       </c>
@@ -4245,8 +4260,8 @@
       </c>
       <c r="G105" s="82"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="131"/>
+    <row r="106" spans="1:7" ht="18">
+      <c r="A106" s="128"/>
       <c r="B106" s="8" t="s">
         <v>6</v>
       </c>
@@ -4264,8 +4279,8 @@
       </c>
       <c r="G106" s="82"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="131"/>
+    <row r="107" spans="1:7" ht="18">
+      <c r="A107" s="128"/>
       <c r="B107" s="8" t="s">
         <v>7</v>
       </c>
@@ -4275,8 +4290,8 @@
       <c r="F107" s="42"/>
       <c r="G107" s="82"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="131"/>
+    <row r="108" spans="1:7" ht="18">
+      <c r="A108" s="128"/>
       <c r="B108" s="8" t="s">
         <v>8</v>
       </c>
@@ -4286,8 +4301,8 @@
       <c r="F108" s="42"/>
       <c r="G108" s="82"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="131"/>
+    <row r="109" spans="1:7" ht="18">
+      <c r="A109" s="128"/>
       <c r="B109" s="8" t="s">
         <v>9</v>
       </c>
@@ -4297,8 +4312,8 @@
       <c r="F109" s="42"/>
       <c r="G109" s="82"/>
     </row>
-    <row r="110" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="131"/>
+    <row r="110" spans="1:7" ht="19" thickBot="1">
+      <c r="A110" s="128"/>
       <c r="B110" s="12" t="s">
         <v>10</v>
       </c>
@@ -4308,8 +4323,8 @@
       <c r="F110" s="76"/>
       <c r="G110" s="92"/>
     </row>
-    <row r="111" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="132" t="s">
+    <row r="111" spans="1:7" ht="19" thickTop="1">
+      <c r="A111" s="146" t="s">
         <v>25</v>
       </c>
       <c r="B111" s="14" t="s">
@@ -4329,8 +4344,8 @@
       </c>
       <c r="G111" s="95"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" s="133"/>
+    <row r="112" spans="1:7" ht="18">
+      <c r="A112" s="147"/>
       <c r="B112" s="8" t="s">
         <v>5</v>
       </c>
@@ -4348,8 +4363,8 @@
       </c>
       <c r="G112" s="96"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="133"/>
+    <row r="113" spans="1:7" ht="18">
+      <c r="A113" s="147"/>
       <c r="B113" s="8" t="s">
         <v>6</v>
       </c>
@@ -4367,8 +4382,8 @@
       </c>
       <c r="G113" s="96"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="133"/>
+    <row r="114" spans="1:7" ht="18">
+      <c r="A114" s="147"/>
       <c r="B114" s="8" t="s">
         <v>7</v>
       </c>
@@ -4386,8 +4401,8 @@
       </c>
       <c r="G114" s="96"/>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A115" s="133"/>
+    <row r="115" spans="1:7" ht="32">
+      <c r="A115" s="147"/>
       <c r="B115" s="8" t="s">
         <v>8</v>
       </c>
@@ -4407,8 +4422,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="133"/>
+    <row r="116" spans="1:7" ht="18">
+      <c r="A116" s="147"/>
       <c r="B116" s="8" t="s">
         <v>9</v>
       </c>
@@ -4426,8 +4441,8 @@
       </c>
       <c r="G116" s="96"/>
     </row>
-    <row r="117" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="134"/>
+    <row r="117" spans="1:7" ht="19" thickBot="1">
+      <c r="A117" s="148"/>
       <c r="B117" s="11" t="s">
         <v>10</v>
       </c>
@@ -4445,8 +4460,8 @@
       </c>
       <c r="G117" s="97"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="135" t="s">
+    <row r="118" spans="1:7" ht="18">
+      <c r="A118" s="149" t="s">
         <v>26</v>
       </c>
       <c r="B118" s="6" t="s">
@@ -4462,8 +4477,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="136"/>
+    <row r="119" spans="1:7" ht="18">
+      <c r="A119" s="150"/>
       <c r="B119" s="8" t="s">
         <v>5</v>
       </c>
@@ -4475,8 +4490,8 @@
       <c r="F119" s="49"/>
       <c r="G119" s="96"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="136"/>
+    <row r="120" spans="1:7" ht="18">
+      <c r="A120" s="150"/>
       <c r="B120" s="8" t="s">
         <v>6</v>
       </c>
@@ -4486,8 +4501,8 @@
       <c r="F120" s="49"/>
       <c r="G120" s="96"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="136"/>
+    <row r="121" spans="1:7" ht="18">
+      <c r="A121" s="150"/>
       <c r="B121" s="8" t="s">
         <v>7</v>
       </c>
@@ -4497,8 +4512,8 @@
       <c r="F121" s="49"/>
       <c r="G121" s="96"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="136"/>
+    <row r="122" spans="1:7" ht="18">
+      <c r="A122" s="150"/>
       <c r="B122" s="8" t="s">
         <v>8</v>
       </c>
@@ -4508,8 +4523,8 @@
       <c r="F122" s="49"/>
       <c r="G122" s="96"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="136"/>
+    <row r="123" spans="1:7" ht="18">
+      <c r="A123" s="150"/>
       <c r="B123" s="8" t="s">
         <v>9</v>
       </c>
@@ -4519,8 +4534,8 @@
       <c r="F123" s="49"/>
       <c r="G123" s="96"/>
     </row>
-    <row r="124" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="137"/>
+    <row r="124" spans="1:7" ht="19" thickBot="1">
+      <c r="A124" s="151"/>
       <c r="B124" s="11" t="s">
         <v>10</v>
       </c>
@@ -4530,8 +4545,8 @@
       <c r="F124" s="59"/>
       <c r="G124" s="97"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="135" t="s">
+    <row r="125" spans="1:7" ht="18">
+      <c r="A125" s="149" t="s">
         <v>27</v>
       </c>
       <c r="B125" s="6" t="s">
@@ -4551,8 +4566,8 @@
       </c>
       <c r="G125" s="98"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="136"/>
+    <row r="126" spans="1:7" ht="18">
+      <c r="A126" s="150"/>
       <c r="B126" s="8" t="s">
         <v>5</v>
       </c>
@@ -4570,8 +4585,8 @@
       </c>
       <c r="G126" s="96"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="136"/>
+    <row r="127" spans="1:7" ht="18">
+      <c r="A127" s="150"/>
       <c r="B127" s="8" t="s">
         <v>6</v>
       </c>
@@ -4589,8 +4604,8 @@
       </c>
       <c r="G127" s="96"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="136"/>
+    <row r="128" spans="1:7" ht="18">
+      <c r="A128" s="150"/>
       <c r="B128" s="8" t="s">
         <v>7</v>
       </c>
@@ -4600,8 +4615,8 @@
       <c r="F128" s="42"/>
       <c r="G128" s="96"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="136"/>
+    <row r="129" spans="1:7" ht="18">
+      <c r="A129" s="150"/>
       <c r="B129" s="8" t="s">
         <v>8</v>
       </c>
@@ -4611,8 +4626,8 @@
       <c r="F129" s="42"/>
       <c r="G129" s="96"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="136"/>
+    <row r="130" spans="1:7" ht="18">
+      <c r="A130" s="150"/>
       <c r="B130" s="8" t="s">
         <v>9</v>
       </c>
@@ -4622,8 +4637,8 @@
       <c r="F130" s="42"/>
       <c r="G130" s="96"/>
     </row>
-    <row r="131" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="138"/>
+    <row r="131" spans="1:7" ht="19" thickBot="1">
+      <c r="A131" s="152"/>
       <c r="B131" s="15" t="s">
         <v>10</v>
       </c>
@@ -4641,8 +4656,8 @@
       </c>
       <c r="G131" s="101"/>
     </row>
-    <row r="132" spans="1:7" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="128" t="s">
+    <row r="132" spans="1:7" ht="19" thickTop="1">
+      <c r="A132" s="144" t="s">
         <v>28</v>
       </c>
       <c r="B132" s="16" t="s">
@@ -4662,8 +4677,8 @@
       </c>
       <c r="G132" s="103"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="128"/>
+    <row r="133" spans="1:7" ht="18">
+      <c r="A133" s="144"/>
       <c r="B133" s="8" t="s">
         <v>5</v>
       </c>
@@ -4681,8 +4696,8 @@
       </c>
       <c r="G133" s="42"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="128"/>
+    <row r="134" spans="1:7" ht="18">
+      <c r="A134" s="144"/>
       <c r="B134" s="8" t="s">
         <v>6</v>
       </c>
@@ -4700,8 +4715,8 @@
       </c>
       <c r="G134" s="42"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" s="128"/>
+    <row r="135" spans="1:7" ht="18">
+      <c r="A135" s="144"/>
       <c r="B135" s="8" t="s">
         <v>7</v>
       </c>
@@ -4719,8 +4734,8 @@
       </c>
       <c r="G135" s="42"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" s="128"/>
+    <row r="136" spans="1:7" ht="18">
+      <c r="A136" s="144"/>
       <c r="B136" s="8" t="s">
         <v>8</v>
       </c>
@@ -4730,8 +4745,8 @@
       <c r="F136" s="42"/>
       <c r="G136" s="42"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" s="128"/>
+    <row r="137" spans="1:7" ht="18">
+      <c r="A137" s="144"/>
       <c r="B137" s="8" t="s">
         <v>9</v>
       </c>
@@ -4741,8 +4756,8 @@
       <c r="F137" s="42"/>
       <c r="G137" s="42"/>
     </row>
-    <row r="138" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="129"/>
+    <row r="138" spans="1:7" ht="19" thickBot="1">
+      <c r="A138" s="145"/>
       <c r="B138" s="11" t="s">
         <v>10</v>
       </c>
@@ -4752,8 +4767,8 @@
       <c r="F138" s="83"/>
       <c r="G138" s="83"/>
     </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A139" s="127" t="s">
+    <row r="139" spans="1:7" ht="32">
+      <c r="A139" s="143" t="s">
         <v>31</v>
       </c>
       <c r="B139" s="6" t="s">
@@ -4767,8 +4782,8 @@
       <c r="F139" s="46"/>
       <c r="G139" s="68"/>
     </row>
-    <row r="140" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="128"/>
+    <row r="140" spans="1:7" ht="19" thickBot="1">
+      <c r="A140" s="144"/>
       <c r="B140" s="8" t="s">
         <v>5</v>
       </c>
@@ -4780,8 +4795,8 @@
       <c r="F140" s="49"/>
       <c r="G140" s="42"/>
     </row>
-    <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A141" s="128"/>
+    <row r="141" spans="1:7" ht="32">
+      <c r="A141" s="144"/>
       <c r="B141" s="8" t="s">
         <v>6</v>
       </c>
@@ -4797,8 +4812,8 @@
       <c r="F141" s="49"/>
       <c r="G141" s="42"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="128"/>
+    <row r="142" spans="1:7" ht="18">
+      <c r="A142" s="144"/>
       <c r="B142" s="8" t="s">
         <v>7</v>
       </c>
@@ -4810,8 +4825,8 @@
       <c r="F142" s="49"/>
       <c r="G142" s="42"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" s="128"/>
+    <row r="143" spans="1:7" ht="18">
+      <c r="A143" s="144"/>
       <c r="B143" s="8" t="s">
         <v>8</v>
       </c>
@@ -4823,8 +4838,8 @@
       <c r="F143" s="49"/>
       <c r="G143" s="42"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" s="128"/>
+    <row r="144" spans="1:7" ht="18">
+      <c r="A144" s="144"/>
       <c r="B144" s="8" t="s">
         <v>9</v>
       </c>
@@ -4836,8 +4851,8 @@
       <c r="F144" s="49"/>
       <c r="G144" s="42"/>
     </row>
-    <row r="145" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="129"/>
+    <row r="145" spans="1:7" ht="19" thickBot="1">
+      <c r="A145" s="145"/>
       <c r="B145" s="11" t="s">
         <v>10</v>
       </c>
@@ -4849,8 +4864,8 @@
       <c r="F145" s="59"/>
       <c r="G145" s="83"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="127" t="s">
+    <row r="146" spans="1:7" ht="18">
+      <c r="A146" s="143" t="s">
         <v>29</v>
       </c>
       <c r="B146" s="6" t="s">
@@ -4864,8 +4879,8 @@
       <c r="F146" s="46"/>
       <c r="G146" s="68"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="128"/>
+    <row r="147" spans="1:7" ht="18">
+      <c r="A147" s="144"/>
       <c r="B147" s="8" t="s">
         <v>5</v>
       </c>
@@ -4877,8 +4892,8 @@
       <c r="F147" s="49"/>
       <c r="G147" s="42"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="128"/>
+    <row r="148" spans="1:7" ht="18">
+      <c r="A148" s="144"/>
       <c r="B148" s="8" t="s">
         <v>6</v>
       </c>
@@ -4890,8 +4905,8 @@
       <c r="F148" s="49"/>
       <c r="G148" s="42"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="128"/>
+    <row r="149" spans="1:7" ht="18">
+      <c r="A149" s="144"/>
       <c r="B149" s="8" t="s">
         <v>7</v>
       </c>
@@ -4903,8 +4918,8 @@
       <c r="F149" s="49"/>
       <c r="G149" s="42"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="128"/>
+    <row r="150" spans="1:7" ht="18">
+      <c r="A150" s="144"/>
       <c r="B150" s="8" t="s">
         <v>8</v>
       </c>
@@ -4914,8 +4929,8 @@
       <c r="F150" s="49"/>
       <c r="G150" s="42"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="128"/>
+    <row r="151" spans="1:7" ht="18">
+      <c r="A151" s="144"/>
       <c r="B151" s="8" t="s">
         <v>9</v>
       </c>
@@ -4927,8 +4942,8 @@
       <c r="F151" s="49"/>
       <c r="G151" s="42"/>
     </row>
-    <row r="152" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="129"/>
+    <row r="152" spans="1:7" ht="19" thickBot="1">
+      <c r="A152" s="145"/>
       <c r="B152" s="11" t="s">
         <v>10</v>
       </c>
@@ -4940,8 +4955,20 @@
       <c r="F152" s="59"/>
       <c r="G152" s="83"/>
     </row>
+    <row r="159" spans="1:7">
+      <c r="C159" s="153" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A146:A152"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A125:A131"/>
+    <mergeCell ref="A132:A138"/>
+    <mergeCell ref="A139:A145"/>
     <mergeCell ref="A97:A103"/>
     <mergeCell ref="A5:A11"/>
     <mergeCell ref="A12:A18"/>
@@ -4956,39 +4983,35 @@
     <mergeCell ref="A41:A47"/>
     <mergeCell ref="A90:A96"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A146:A152"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A125:A131"/>
-    <mergeCell ref="A132:A138"/>
-    <mergeCell ref="A139:A145"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C159" r:id="rId1" xr:uid="{E53A9555-6A20-3843-B157-6085AF83AF9B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
* https://stackoverflow.com/questions/55586138/how-to-get-the-values-from-a-multiple-search-selection-dropdown-box-in-react-sem https://embed.plnkr.co/plunk/FvOiuo https://codesandbox.io/s/mjnyx49vj9?from-embed
</commit_message>
<xml_diff>
--- a/190503StartseitenkonzeptB.xlsx
+++ b/190503StartseitenkonzeptB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lc_admin.planks/Documents/ttt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090351AE-1072-6545-BB17-DB0076079934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D0CF72-E655-184F-A790-1434D4059A2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1642,12 +1642,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1690,37 +1721,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2622,7 +2622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C147" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
@@ -2630,7 +2630,7 @@
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
-    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="30.5" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="41.33203125" customWidth="1"/>
     <col min="6" max="6" width="33.6640625" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
@@ -2700,7 +2700,7 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="141" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2722,7 +2722,7 @@
       <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="18">
-      <c r="A6" s="131"/>
+      <c r="A6" s="142"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="52.5" customHeight="1">
-      <c r="A7" s="131"/>
+      <c r="A7" s="142"/>
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
@@ -2764,7 +2764,7 @@
       <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="18">
-      <c r="A8" s="131"/>
+      <c r="A8" s="142"/>
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="18">
-      <c r="A9" s="131"/>
+      <c r="A9" s="142"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" ht="18">
-      <c r="A10" s="131"/>
+      <c r="A10" s="142"/>
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="19" thickBot="1">
-      <c r="A11" s="132"/>
+      <c r="A11" s="143"/>
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
@@ -2844,7 +2844,7 @@
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" ht="32">
-      <c r="A12" s="130" t="s">
+      <c r="A12" s="141" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -2865,7 +2865,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
-      <c r="A13" s="131"/>
+      <c r="A13" s="142"/>
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
@@ -2882,7 +2882,7 @@
       <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A14" s="131"/>
+      <c r="A14" s="142"/>
       <c r="B14" s="8" t="s">
         <v>6</v>
       </c>
@@ -2899,7 +2899,7 @@
       <c r="G14" s="50"/>
     </row>
     <row r="15" spans="1:8" ht="18">
-      <c r="A15" s="131"/>
+      <c r="A15" s="142"/>
       <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" ht="18">
-      <c r="A16" s="131"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:8" ht="18">
-      <c r="A17" s="131"/>
+      <c r="A17" s="142"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -2952,7 +2952,7 @@
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="19" thickBot="1">
-      <c r="A18" s="132"/>
+      <c r="A18" s="143"/>
       <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
@@ -2990,7 +2990,7 @@
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8" ht="32">
-      <c r="A20" s="130" t="s">
+      <c r="A20" s="141" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -3006,7 +3006,7 @@
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A21" s="133"/>
+      <c r="A21" s="144"/>
       <c r="B21" s="8" t="s">
         <v>5</v>
       </c>
@@ -3019,7 +3019,7 @@
       <c r="G21" s="50"/>
     </row>
     <row r="22" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A22" s="133"/>
+      <c r="A22" s="144"/>
       <c r="B22" s="8" t="s">
         <v>6</v>
       </c>
@@ -3032,7 +3032,7 @@
       <c r="G22" s="50"/>
     </row>
     <row r="23" spans="1:8" ht="32">
-      <c r="A23" s="133"/>
+      <c r="A23" s="144"/>
       <c r="B23" s="8" t="s">
         <v>7</v>
       </c>
@@ -3045,7 +3045,7 @@
       <c r="G23" s="50"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A24" s="133"/>
+      <c r="A24" s="144"/>
       <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
@@ -3058,7 +3058,7 @@
       <c r="G24" s="50"/>
     </row>
     <row r="25" spans="1:8" ht="32">
-      <c r="A25" s="133"/>
+      <c r="A25" s="144"/>
       <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
@@ -3071,7 +3071,7 @@
       <c r="G25" s="50"/>
     </row>
     <row r="26" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A26" s="134"/>
+      <c r="A26" s="145"/>
       <c r="B26" s="12" t="s">
         <v>10</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="G26" s="77"/>
     </row>
     <row r="27" spans="1:8" ht="36.75" customHeight="1">
-      <c r="A27" s="136" t="s">
+      <c r="A27" s="147" t="s">
         <v>85</v>
       </c>
       <c r="B27" s="6" t="s">
@@ -3106,7 +3106,7 @@
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8" ht="18">
-      <c r="A28" s="137"/>
+      <c r="A28" s="148"/>
       <c r="B28" s="8" t="s">
         <v>5</v>
       </c>
@@ -3123,7 +3123,7 @@
       <c r="G28" s="50"/>
     </row>
     <row r="29" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A29" s="137"/>
+      <c r="A29" s="148"/>
       <c r="B29" s="8" t="s">
         <v>6</v>
       </c>
@@ -3140,7 +3140,7 @@
       <c r="G29" s="50"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A30" s="137"/>
+      <c r="A30" s="148"/>
       <c r="B30" s="8" t="s">
         <v>7</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="G30" s="50"/>
     </row>
     <row r="31" spans="1:8" ht="18">
-      <c r="A31" s="137"/>
+      <c r="A31" s="148"/>
       <c r="B31" s="8" t="s">
         <v>8</v>
       </c>
@@ -3174,7 +3174,7 @@
       <c r="G31" s="50"/>
     </row>
     <row r="32" spans="1:8" ht="82.5" customHeight="1">
-      <c r="A32" s="137"/>
+      <c r="A32" s="148"/>
       <c r="B32" s="8" t="s">
         <v>9</v>
       </c>
@@ -3191,7 +3191,7 @@
       <c r="G32" s="50"/>
     </row>
     <row r="33" spans="1:8" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A33" s="137"/>
+      <c r="A33" s="148"/>
       <c r="B33" s="12" t="s">
         <v>10</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="G33" s="77"/>
     </row>
     <row r="34" spans="1:8" ht="33" thickTop="1">
-      <c r="A34" s="136" t="s">
+      <c r="A34" s="147" t="s">
         <v>100</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -3224,7 +3224,7 @@
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A35" s="141"/>
+      <c r="A35" s="152"/>
       <c r="B35" s="8" t="s">
         <v>5</v>
       </c>
@@ -3237,7 +3237,7 @@
       <c r="G35" s="50"/>
     </row>
     <row r="36" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A36" s="141"/>
+      <c r="A36" s="152"/>
       <c r="B36" s="8" t="s">
         <v>6</v>
       </c>
@@ -3250,7 +3250,7 @@
       <c r="G36" s="50"/>
     </row>
     <row r="37" spans="1:8" ht="18">
-      <c r="A37" s="141"/>
+      <c r="A37" s="152"/>
       <c r="B37" s="8" t="s">
         <v>7</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="G37" s="50"/>
     </row>
     <row r="38" spans="1:8" ht="16.5" customHeight="1">
-      <c r="A38" s="141"/>
+      <c r="A38" s="152"/>
       <c r="B38" s="8" t="s">
         <v>8</v>
       </c>
@@ -3276,7 +3276,7 @@
       <c r="G38" s="50"/>
     </row>
     <row r="39" spans="1:8" ht="64">
-      <c r="A39" s="141"/>
+      <c r="A39" s="152"/>
       <c r="B39" s="8" t="s">
         <v>9</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="G39" s="50"/>
     </row>
     <row r="40" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A40" s="142"/>
+      <c r="A40" s="153"/>
       <c r="B40" s="12" t="s">
         <v>10</v>
       </c>
@@ -3302,7 +3302,7 @@
       <c r="G40" s="77"/>
     </row>
     <row r="41" spans="1:8" ht="32">
-      <c r="A41" s="136" t="s">
+      <c r="A41" s="147" t="s">
         <v>82</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -3320,7 +3320,7 @@
       <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8" ht="18">
-      <c r="A42" s="137"/>
+      <c r="A42" s="148"/>
       <c r="B42" s="8" t="s">
         <v>5</v>
       </c>
@@ -3335,7 +3335,7 @@
       <c r="G42" s="50"/>
     </row>
     <row r="43" spans="1:8" ht="32">
-      <c r="A43" s="137"/>
+      <c r="A43" s="148"/>
       <c r="B43" s="8" t="s">
         <v>6</v>
       </c>
@@ -3350,7 +3350,7 @@
       <c r="G43" s="50"/>
     </row>
     <row r="44" spans="1:8" ht="18">
-      <c r="A44" s="137"/>
+      <c r="A44" s="148"/>
       <c r="B44" s="8" t="s">
         <v>7</v>
       </c>
@@ -3365,7 +3365,7 @@
       <c r="G44" s="50"/>
     </row>
     <row r="45" spans="1:8" ht="18">
-      <c r="A45" s="137"/>
+      <c r="A45" s="148"/>
       <c r="B45" s="8" t="s">
         <v>8</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="G45" s="50"/>
     </row>
     <row r="46" spans="1:8" ht="48">
-      <c r="A46" s="137"/>
+      <c r="A46" s="148"/>
       <c r="B46" s="8" t="s">
         <v>9</v>
       </c>
@@ -3395,7 +3395,7 @@
       <c r="G46" s="38"/>
     </row>
     <row r="47" spans="1:8" ht="19" thickBot="1">
-      <c r="A47" s="137"/>
+      <c r="A47" s="148"/>
       <c r="B47" s="12" t="s">
         <v>10</v>
       </c>
@@ -3410,7 +3410,7 @@
       <c r="G47" s="77"/>
     </row>
     <row r="48" spans="1:8" ht="33" thickTop="1">
-      <c r="A48" s="136" t="s">
+      <c r="A48" s="147" t="s">
         <v>114</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -3432,7 +3432,7 @@
       <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:7" ht="18">
-      <c r="A49" s="137"/>
+      <c r="A49" s="148"/>
       <c r="B49" s="8" t="s">
         <v>5</v>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="G49" s="50"/>
     </row>
     <row r="50" spans="1:7" ht="93.75" customHeight="1">
-      <c r="A50" s="137"/>
+      <c r="A50" s="148"/>
       <c r="B50" s="8" t="s">
         <v>6</v>
       </c>
@@ -3466,7 +3466,7 @@
       <c r="G50" s="50"/>
     </row>
     <row r="51" spans="1:7" ht="18">
-      <c r="A51" s="137"/>
+      <c r="A51" s="148"/>
       <c r="B51" s="8" t="s">
         <v>7</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="G51" s="50"/>
     </row>
     <row r="52" spans="1:7" ht="18">
-      <c r="A52" s="137"/>
+      <c r="A52" s="148"/>
       <c r="B52" s="8" t="s">
         <v>8</v>
       </c>
@@ -3500,7 +3500,7 @@
       <c r="G52" s="50"/>
     </row>
     <row r="53" spans="1:7" ht="65.25" customHeight="1">
-      <c r="A53" s="137"/>
+      <c r="A53" s="148"/>
       <c r="B53" s="8" t="s">
         <v>9</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="G53" s="50"/>
     </row>
     <row r="54" spans="1:7" ht="19" thickBot="1">
-      <c r="A54" s="137"/>
+      <c r="A54" s="148"/>
       <c r="B54" s="12" t="s">
         <v>10</v>
       </c>
@@ -3534,7 +3534,7 @@
       <c r="G54" s="77"/>
     </row>
     <row r="55" spans="1:7" ht="19" thickTop="1">
-      <c r="A55" s="135" t="s">
+      <c r="A55" s="146" t="s">
         <v>18</v>
       </c>
       <c r="B55" s="13" t="s">
@@ -3549,7 +3549,7 @@
       <c r="G55" s="81"/>
     </row>
     <row r="56" spans="1:7" ht="18">
-      <c r="A56" s="128"/>
+      <c r="A56" s="132"/>
       <c r="B56" s="8" t="s">
         <v>5</v>
       </c>
@@ -3560,7 +3560,7 @@
       <c r="G56" s="82"/>
     </row>
     <row r="57" spans="1:7" ht="18">
-      <c r="A57" s="128"/>
+      <c r="A57" s="132"/>
       <c r="B57" s="8" t="s">
         <v>6</v>
       </c>
@@ -3571,7 +3571,7 @@
       <c r="G57" s="82"/>
     </row>
     <row r="58" spans="1:7" ht="18">
-      <c r="A58" s="128"/>
+      <c r="A58" s="132"/>
       <c r="B58" s="8" t="s">
         <v>7</v>
       </c>
@@ -3582,7 +3582,7 @@
       <c r="G58" s="82"/>
     </row>
     <row r="59" spans="1:7" ht="18">
-      <c r="A59" s="128"/>
+      <c r="A59" s="132"/>
       <c r="B59" s="8" t="s">
         <v>8</v>
       </c>
@@ -3593,7 +3593,7 @@
       <c r="G59" s="82"/>
     </row>
     <row r="60" spans="1:7" ht="18">
-      <c r="A60" s="128"/>
+      <c r="A60" s="132"/>
       <c r="B60" s="8" t="s">
         <v>9</v>
       </c>
@@ -3604,7 +3604,7 @@
       <c r="G60" s="82"/>
     </row>
     <row r="61" spans="1:7" ht="19" thickBot="1">
-      <c r="A61" s="129"/>
+      <c r="A61" s="140"/>
       <c r="B61" s="11" t="s">
         <v>10</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="G61" s="84"/>
     </row>
     <row r="62" spans="1:7" ht="32">
-      <c r="A62" s="127" t="s">
+      <c r="A62" s="131" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="6" t="s">
@@ -3634,7 +3634,7 @@
       <c r="G62" s="85"/>
     </row>
     <row r="63" spans="1:7" ht="18">
-      <c r="A63" s="128"/>
+      <c r="A63" s="132"/>
       <c r="B63" s="8" t="s">
         <v>5</v>
       </c>
@@ -3645,7 +3645,7 @@
       <c r="G63" s="82"/>
     </row>
     <row r="64" spans="1:7" ht="18">
-      <c r="A64" s="128"/>
+      <c r="A64" s="132"/>
       <c r="B64" s="8" t="s">
         <v>6</v>
       </c>
@@ -3662,7 +3662,7 @@
       <c r="G64" s="82"/>
     </row>
     <row r="65" spans="1:7" ht="18">
-      <c r="A65" s="128"/>
+      <c r="A65" s="132"/>
       <c r="B65" s="8" t="s">
         <v>7</v>
       </c>
@@ -3673,7 +3673,7 @@
       <c r="G65" s="82"/>
     </row>
     <row r="66" spans="1:7" ht="18">
-      <c r="A66" s="128"/>
+      <c r="A66" s="132"/>
       <c r="B66" s="8" t="s">
         <v>8</v>
       </c>
@@ -3684,7 +3684,7 @@
       <c r="G66" s="82"/>
     </row>
     <row r="67" spans="1:7" ht="18">
-      <c r="A67" s="128"/>
+      <c r="A67" s="132"/>
       <c r="B67" s="8" t="s">
         <v>9</v>
       </c>
@@ -3695,7 +3695,7 @@
       <c r="G67" s="82"/>
     </row>
     <row r="68" spans="1:7" ht="19" thickBot="1">
-      <c r="A68" s="129"/>
+      <c r="A68" s="140"/>
       <c r="B68" s="11" t="s">
         <v>10</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="G68" s="84"/>
     </row>
     <row r="69" spans="1:7" ht="18">
-      <c r="A69" s="127" t="s">
+      <c r="A69" s="131" t="s">
         <v>20</v>
       </c>
       <c r="B69" s="6" t="s">
@@ -3723,7 +3723,7 @@
       <c r="G69" s="85"/>
     </row>
     <row r="70" spans="1:7" ht="18">
-      <c r="A70" s="128"/>
+      <c r="A70" s="132"/>
       <c r="B70" s="8" t="s">
         <v>5</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="G70" s="82"/>
     </row>
     <row r="71" spans="1:7" ht="18">
-      <c r="A71" s="128"/>
+      <c r="A71" s="132"/>
       <c r="B71" s="8" t="s">
         <v>6</v>
       </c>
@@ -3747,7 +3747,7 @@
       <c r="G71" s="82"/>
     </row>
     <row r="72" spans="1:7" ht="18">
-      <c r="A72" s="128"/>
+      <c r="A72" s="132"/>
       <c r="B72" s="8" t="s">
         <v>7</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="G72" s="82"/>
     </row>
     <row r="73" spans="1:7" ht="18">
-      <c r="A73" s="128"/>
+      <c r="A73" s="132"/>
       <c r="B73" s="8" t="s">
         <v>8</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="G73" s="82"/>
     </row>
     <row r="74" spans="1:7" ht="18">
-      <c r="A74" s="128"/>
+      <c r="A74" s="132"/>
       <c r="B74" s="8" t="s">
         <v>9</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="G74" s="82"/>
     </row>
     <row r="75" spans="1:7" ht="19" thickBot="1">
-      <c r="A75" s="129"/>
+      <c r="A75" s="140"/>
       <c r="B75" s="11" t="s">
         <v>10</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="G75" s="84"/>
     </row>
     <row r="76" spans="1:7" ht="18">
-      <c r="A76" s="127" t="s">
+      <c r="A76" s="131" t="s">
         <v>21</v>
       </c>
       <c r="B76" s="6" t="s">
@@ -3806,7 +3806,7 @@
       <c r="G76" s="85"/>
     </row>
     <row r="77" spans="1:7" ht="18">
-      <c r="A77" s="128"/>
+      <c r="A77" s="132"/>
       <c r="B77" s="8" t="s">
         <v>5</v>
       </c>
@@ -3817,7 +3817,7 @@
       <c r="G77" s="82"/>
     </row>
     <row r="78" spans="1:7" ht="18">
-      <c r="A78" s="128"/>
+      <c r="A78" s="132"/>
       <c r="B78" s="8" t="s">
         <v>6</v>
       </c>
@@ -3828,7 +3828,7 @@
       <c r="G78" s="82"/>
     </row>
     <row r="79" spans="1:7" ht="18">
-      <c r="A79" s="128"/>
+      <c r="A79" s="132"/>
       <c r="B79" s="8" t="s">
         <v>7</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="G79" s="82"/>
     </row>
     <row r="80" spans="1:7" ht="18">
-      <c r="A80" s="128"/>
+      <c r="A80" s="132"/>
       <c r="B80" s="8" t="s">
         <v>8</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="G80" s="82"/>
     </row>
     <row r="81" spans="1:7" ht="18">
-      <c r="A81" s="128"/>
+      <c r="A81" s="132"/>
       <c r="B81" s="8" t="s">
         <v>9</v>
       </c>
@@ -3861,7 +3861,7 @@
       <c r="G81" s="82"/>
     </row>
     <row r="82" spans="1:7" ht="19" thickBot="1">
-      <c r="A82" s="129"/>
+      <c r="A82" s="140"/>
       <c r="B82" s="11" t="s">
         <v>10</v>
       </c>
@@ -3872,7 +3872,7 @@
       <c r="G82" s="84"/>
     </row>
     <row r="83" spans="1:7" ht="64">
-      <c r="A83" s="127" t="s">
+      <c r="A83" s="131" t="s">
         <v>22</v>
       </c>
       <c r="B83" s="6" t="s">
@@ -3893,7 +3893,7 @@
       <c r="G83" s="85"/>
     </row>
     <row r="84" spans="1:7" ht="18">
-      <c r="A84" s="128"/>
+      <c r="A84" s="132"/>
       <c r="B84" s="8" t="s">
         <v>5</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="G84" s="82"/>
     </row>
     <row r="85" spans="1:7" ht="48">
-      <c r="A85" s="128"/>
+      <c r="A85" s="132"/>
       <c r="B85" s="8" t="s">
         <v>6</v>
       </c>
@@ -3931,7 +3931,7 @@
       <c r="G85" s="82"/>
     </row>
     <row r="86" spans="1:7" ht="18">
-      <c r="A86" s="128"/>
+      <c r="A86" s="132"/>
       <c r="B86" s="8" t="s">
         <v>7</v>
       </c>
@@ -3950,7 +3950,7 @@
       <c r="G86" s="82"/>
     </row>
     <row r="87" spans="1:7" ht="32">
-      <c r="A87" s="128"/>
+      <c r="A87" s="132"/>
       <c r="B87" s="8" t="s">
         <v>8</v>
       </c>
@@ -3969,7 +3969,7 @@
       <c r="G87" s="82"/>
     </row>
     <row r="88" spans="1:7" ht="32">
-      <c r="A88" s="128"/>
+      <c r="A88" s="132"/>
       <c r="B88" s="8" t="s">
         <v>9</v>
       </c>
@@ -3988,7 +3988,7 @@
       <c r="G88" s="82"/>
     </row>
     <row r="89" spans="1:7" ht="19" thickBot="1">
-      <c r="A89" s="129"/>
+      <c r="A89" s="140"/>
       <c r="B89" s="11" t="s">
         <v>10</v>
       </c>
@@ -4007,7 +4007,7 @@
       <c r="G89" s="84"/>
     </row>
     <row r="90" spans="1:7" ht="48">
-      <c r="A90" s="138" t="s">
+      <c r="A90" s="149" t="s">
         <v>86</v>
       </c>
       <c r="B90" s="6" t="s">
@@ -4026,7 +4026,7 @@
       <c r="G90" s="85"/>
     </row>
     <row r="91" spans="1:7" ht="18">
-      <c r="A91" s="139"/>
+      <c r="A91" s="150"/>
       <c r="B91" s="8" t="s">
         <v>5</v>
       </c>
@@ -4043,7 +4043,7 @@
       <c r="G91" s="82"/>
     </row>
     <row r="92" spans="1:7" ht="18">
-      <c r="A92" s="139"/>
+      <c r="A92" s="150"/>
       <c r="B92" s="8" t="s">
         <v>6</v>
       </c>
@@ -4060,7 +4060,7 @@
       <c r="G92" s="82"/>
     </row>
     <row r="93" spans="1:7" ht="18">
-      <c r="A93" s="139"/>
+      <c r="A93" s="150"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="G93" s="82"/>
     </row>
     <row r="94" spans="1:7" ht="18">
-      <c r="A94" s="139"/>
+      <c r="A94" s="150"/>
       <c r="B94" s="8" t="s">
         <v>8</v>
       </c>
@@ -4094,7 +4094,7 @@
       <c r="G94" s="82"/>
     </row>
     <row r="95" spans="1:7" ht="18">
-      <c r="A95" s="139"/>
+      <c r="A95" s="150"/>
       <c r="B95" s="8" t="s">
         <v>9</v>
       </c>
@@ -4111,7 +4111,7 @@
       <c r="G95" s="82"/>
     </row>
     <row r="96" spans="1:7" ht="19" thickBot="1">
-      <c r="A96" s="140"/>
+      <c r="A96" s="151"/>
       <c r="B96" s="11" t="s">
         <v>10</v>
       </c>
@@ -4128,7 +4128,7 @@
       <c r="G96" s="84"/>
     </row>
     <row r="97" spans="1:7" ht="32">
-      <c r="A97" s="127" t="s">
+      <c r="A97" s="131" t="s">
         <v>23</v>
       </c>
       <c r="B97" s="6" t="s">
@@ -4143,7 +4143,7 @@
       <c r="G97" s="85"/>
     </row>
     <row r="98" spans="1:7" ht="18">
-      <c r="A98" s="128"/>
+      <c r="A98" s="132"/>
       <c r="B98" s="8" t="s">
         <v>5</v>
       </c>
@@ -4156,7 +4156,7 @@
       <c r="G98" s="82"/>
     </row>
     <row r="99" spans="1:7" ht="18">
-      <c r="A99" s="128"/>
+      <c r="A99" s="132"/>
       <c r="B99" s="8" t="s">
         <v>6</v>
       </c>
@@ -4169,7 +4169,7 @@
       <c r="G99" s="82"/>
     </row>
     <row r="100" spans="1:7" ht="18">
-      <c r="A100" s="128"/>
+      <c r="A100" s="132"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
       </c>
@@ -4182,7 +4182,7 @@
       <c r="G100" s="82"/>
     </row>
     <row r="101" spans="1:7" ht="18">
-      <c r="A101" s="128"/>
+      <c r="A101" s="132"/>
       <c r="B101" s="8" t="s">
         <v>8</v>
       </c>
@@ -4195,7 +4195,7 @@
       <c r="G101" s="82"/>
     </row>
     <row r="102" spans="1:7" ht="18">
-      <c r="A102" s="128"/>
+      <c r="A102" s="132"/>
       <c r="B102" s="8" t="s">
         <v>9</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="G102" s="82"/>
     </row>
     <row r="103" spans="1:7" ht="19" thickBot="1">
-      <c r="A103" s="129"/>
+      <c r="A103" s="140"/>
       <c r="B103" s="11" t="s">
         <v>10</v>
       </c>
@@ -4221,7 +4221,7 @@
       <c r="G103" s="84"/>
     </row>
     <row r="104" spans="1:7" ht="18">
-      <c r="A104" s="127" t="s">
+      <c r="A104" s="131" t="s">
         <v>24</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -4242,7 +4242,7 @@
       <c r="G104" s="85"/>
     </row>
     <row r="105" spans="1:7" ht="18">
-      <c r="A105" s="128"/>
+      <c r="A105" s="132"/>
       <c r="B105" s="8" t="s">
         <v>5</v>
       </c>
@@ -4261,7 +4261,7 @@
       <c r="G105" s="82"/>
     </row>
     <row r="106" spans="1:7" ht="18">
-      <c r="A106" s="128"/>
+      <c r="A106" s="132"/>
       <c r="B106" s="8" t="s">
         <v>6</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="G106" s="82"/>
     </row>
     <row r="107" spans="1:7" ht="18">
-      <c r="A107" s="128"/>
+      <c r="A107" s="132"/>
       <c r="B107" s="8" t="s">
         <v>7</v>
       </c>
@@ -4291,7 +4291,7 @@
       <c r="G107" s="82"/>
     </row>
     <row r="108" spans="1:7" ht="18">
-      <c r="A108" s="128"/>
+      <c r="A108" s="132"/>
       <c r="B108" s="8" t="s">
         <v>8</v>
       </c>
@@ -4302,7 +4302,7 @@
       <c r="G108" s="82"/>
     </row>
     <row r="109" spans="1:7" ht="18">
-      <c r="A109" s="128"/>
+      <c r="A109" s="132"/>
       <c r="B109" s="8" t="s">
         <v>9</v>
       </c>
@@ -4313,7 +4313,7 @@
       <c r="G109" s="82"/>
     </row>
     <row r="110" spans="1:7" ht="19" thickBot="1">
-      <c r="A110" s="128"/>
+      <c r="A110" s="132"/>
       <c r="B110" s="12" t="s">
         <v>10</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="G110" s="92"/>
     </row>
     <row r="111" spans="1:7" ht="19" thickTop="1">
-      <c r="A111" s="146" t="s">
+      <c r="A111" s="133" t="s">
         <v>25</v>
       </c>
       <c r="B111" s="14" t="s">
@@ -4345,7 +4345,7 @@
       <c r="G111" s="95"/>
     </row>
     <row r="112" spans="1:7" ht="18">
-      <c r="A112" s="147"/>
+      <c r="A112" s="134"/>
       <c r="B112" s="8" t="s">
         <v>5</v>
       </c>
@@ -4364,7 +4364,7 @@
       <c r="G112" s="96"/>
     </row>
     <row r="113" spans="1:7" ht="18">
-      <c r="A113" s="147"/>
+      <c r="A113" s="134"/>
       <c r="B113" s="8" t="s">
         <v>6</v>
       </c>
@@ -4383,7 +4383,7 @@
       <c r="G113" s="96"/>
     </row>
     <row r="114" spans="1:7" ht="18">
-      <c r="A114" s="147"/>
+      <c r="A114" s="134"/>
       <c r="B114" s="8" t="s">
         <v>7</v>
       </c>
@@ -4402,7 +4402,7 @@
       <c r="G114" s="96"/>
     </row>
     <row r="115" spans="1:7" ht="32">
-      <c r="A115" s="147"/>
+      <c r="A115" s="134"/>
       <c r="B115" s="8" t="s">
         <v>8</v>
       </c>
@@ -4423,7 +4423,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="18">
-      <c r="A116" s="147"/>
+      <c r="A116" s="134"/>
       <c r="B116" s="8" t="s">
         <v>9</v>
       </c>
@@ -4442,7 +4442,7 @@
       <c r="G116" s="96"/>
     </row>
     <row r="117" spans="1:7" ht="19" thickBot="1">
-      <c r="A117" s="148"/>
+      <c r="A117" s="135"/>
       <c r="B117" s="11" t="s">
         <v>10</v>
       </c>
@@ -4461,7 +4461,7 @@
       <c r="G117" s="97"/>
     </row>
     <row r="118" spans="1:7" ht="18">
-      <c r="A118" s="149" t="s">
+      <c r="A118" s="136" t="s">
         <v>26</v>
       </c>
       <c r="B118" s="6" t="s">
@@ -4478,7 +4478,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="18">
-      <c r="A119" s="150"/>
+      <c r="A119" s="137"/>
       <c r="B119" s="8" t="s">
         <v>5</v>
       </c>
@@ -4491,7 +4491,7 @@
       <c r="G119" s="96"/>
     </row>
     <row r="120" spans="1:7" ht="18">
-      <c r="A120" s="150"/>
+      <c r="A120" s="137"/>
       <c r="B120" s="8" t="s">
         <v>6</v>
       </c>
@@ -4502,7 +4502,7 @@
       <c r="G120" s="96"/>
     </row>
     <row r="121" spans="1:7" ht="18">
-      <c r="A121" s="150"/>
+      <c r="A121" s="137"/>
       <c r="B121" s="8" t="s">
         <v>7</v>
       </c>
@@ -4513,7 +4513,7 @@
       <c r="G121" s="96"/>
     </row>
     <row r="122" spans="1:7" ht="18">
-      <c r="A122" s="150"/>
+      <c r="A122" s="137"/>
       <c r="B122" s="8" t="s">
         <v>8</v>
       </c>
@@ -4524,7 +4524,7 @@
       <c r="G122" s="96"/>
     </row>
     <row r="123" spans="1:7" ht="18">
-      <c r="A123" s="150"/>
+      <c r="A123" s="137"/>
       <c r="B123" s="8" t="s">
         <v>9</v>
       </c>
@@ -4535,7 +4535,7 @@
       <c r="G123" s="96"/>
     </row>
     <row r="124" spans="1:7" ht="19" thickBot="1">
-      <c r="A124" s="151"/>
+      <c r="A124" s="138"/>
       <c r="B124" s="11" t="s">
         <v>10</v>
       </c>
@@ -4546,7 +4546,7 @@
       <c r="G124" s="97"/>
     </row>
     <row r="125" spans="1:7" ht="18">
-      <c r="A125" s="149" t="s">
+      <c r="A125" s="136" t="s">
         <v>27</v>
       </c>
       <c r="B125" s="6" t="s">
@@ -4567,7 +4567,7 @@
       <c r="G125" s="98"/>
     </row>
     <row r="126" spans="1:7" ht="18">
-      <c r="A126" s="150"/>
+      <c r="A126" s="137"/>
       <c r="B126" s="8" t="s">
         <v>5</v>
       </c>
@@ -4586,7 +4586,7 @@
       <c r="G126" s="96"/>
     </row>
     <row r="127" spans="1:7" ht="18">
-      <c r="A127" s="150"/>
+      <c r="A127" s="137"/>
       <c r="B127" s="8" t="s">
         <v>6</v>
       </c>
@@ -4605,7 +4605,7 @@
       <c r="G127" s="96"/>
     </row>
     <row r="128" spans="1:7" ht="18">
-      <c r="A128" s="150"/>
+      <c r="A128" s="137"/>
       <c r="B128" s="8" t="s">
         <v>7</v>
       </c>
@@ -4616,7 +4616,7 @@
       <c r="G128" s="96"/>
     </row>
     <row r="129" spans="1:7" ht="18">
-      <c r="A129" s="150"/>
+      <c r="A129" s="137"/>
       <c r="B129" s="8" t="s">
         <v>8</v>
       </c>
@@ -4627,7 +4627,7 @@
       <c r="G129" s="96"/>
     </row>
     <row r="130" spans="1:7" ht="18">
-      <c r="A130" s="150"/>
+      <c r="A130" s="137"/>
       <c r="B130" s="8" t="s">
         <v>9</v>
       </c>
@@ -4638,7 +4638,7 @@
       <c r="G130" s="96"/>
     </row>
     <row r="131" spans="1:7" ht="19" thickBot="1">
-      <c r="A131" s="152"/>
+      <c r="A131" s="139"/>
       <c r="B131" s="15" t="s">
         <v>10</v>
       </c>
@@ -4657,7 +4657,7 @@
       <c r="G131" s="101"/>
     </row>
     <row r="132" spans="1:7" ht="19" thickTop="1">
-      <c r="A132" s="144" t="s">
+      <c r="A132" s="129" t="s">
         <v>28</v>
       </c>
       <c r="B132" s="16" t="s">
@@ -4678,7 +4678,7 @@
       <c r="G132" s="103"/>
     </row>
     <row r="133" spans="1:7" ht="18">
-      <c r="A133" s="144"/>
+      <c r="A133" s="129"/>
       <c r="B133" s="8" t="s">
         <v>5</v>
       </c>
@@ -4697,7 +4697,7 @@
       <c r="G133" s="42"/>
     </row>
     <row r="134" spans="1:7" ht="18">
-      <c r="A134" s="144"/>
+      <c r="A134" s="129"/>
       <c r="B134" s="8" t="s">
         <v>6</v>
       </c>
@@ -4716,7 +4716,7 @@
       <c r="G134" s="42"/>
     </row>
     <row r="135" spans="1:7" ht="18">
-      <c r="A135" s="144"/>
+      <c r="A135" s="129"/>
       <c r="B135" s="8" t="s">
         <v>7</v>
       </c>
@@ -4735,7 +4735,7 @@
       <c r="G135" s="42"/>
     </row>
     <row r="136" spans="1:7" ht="18">
-      <c r="A136" s="144"/>
+      <c r="A136" s="129"/>
       <c r="B136" s="8" t="s">
         <v>8</v>
       </c>
@@ -4746,7 +4746,7 @@
       <c r="G136" s="42"/>
     </row>
     <row r="137" spans="1:7" ht="18">
-      <c r="A137" s="144"/>
+      <c r="A137" s="129"/>
       <c r="B137" s="8" t="s">
         <v>9</v>
       </c>
@@ -4757,7 +4757,7 @@
       <c r="G137" s="42"/>
     </row>
     <row r="138" spans="1:7" ht="19" thickBot="1">
-      <c r="A138" s="145"/>
+      <c r="A138" s="130"/>
       <c r="B138" s="11" t="s">
         <v>10</v>
       </c>
@@ -4768,7 +4768,7 @@
       <c r="G138" s="83"/>
     </row>
     <row r="139" spans="1:7" ht="32">
-      <c r="A139" s="143" t="s">
+      <c r="A139" s="128" t="s">
         <v>31</v>
       </c>
       <c r="B139" s="6" t="s">
@@ -4783,7 +4783,7 @@
       <c r="G139" s="68"/>
     </row>
     <row r="140" spans="1:7" ht="19" thickBot="1">
-      <c r="A140" s="144"/>
+      <c r="A140" s="129"/>
       <c r="B140" s="8" t="s">
         <v>5</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="G140" s="42"/>
     </row>
     <row r="141" spans="1:7" ht="32">
-      <c r="A141" s="144"/>
+      <c r="A141" s="129"/>
       <c r="B141" s="8" t="s">
         <v>6</v>
       </c>
@@ -4813,7 +4813,7 @@
       <c r="G141" s="42"/>
     </row>
     <row r="142" spans="1:7" ht="18">
-      <c r="A142" s="144"/>
+      <c r="A142" s="129"/>
       <c r="B142" s="8" t="s">
         <v>7</v>
       </c>
@@ -4826,7 +4826,7 @@
       <c r="G142" s="42"/>
     </row>
     <row r="143" spans="1:7" ht="18">
-      <c r="A143" s="144"/>
+      <c r="A143" s="129"/>
       <c r="B143" s="8" t="s">
         <v>8</v>
       </c>
@@ -4839,7 +4839,7 @@
       <c r="G143" s="42"/>
     </row>
     <row r="144" spans="1:7" ht="18">
-      <c r="A144" s="144"/>
+      <c r="A144" s="129"/>
       <c r="B144" s="8" t="s">
         <v>9</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="G144" s="42"/>
     </row>
     <row r="145" spans="1:7" ht="19" thickBot="1">
-      <c r="A145" s="145"/>
+      <c r="A145" s="130"/>
       <c r="B145" s="11" t="s">
         <v>10</v>
       </c>
@@ -4865,7 +4865,7 @@
       <c r="G145" s="83"/>
     </row>
     <row r="146" spans="1:7" ht="18">
-      <c r="A146" s="143" t="s">
+      <c r="A146" s="128" t="s">
         <v>29</v>
       </c>
       <c r="B146" s="6" t="s">
@@ -4880,7 +4880,7 @@
       <c r="G146" s="68"/>
     </row>
     <row r="147" spans="1:7" ht="18">
-      <c r="A147" s="144"/>
+      <c r="A147" s="129"/>
       <c r="B147" s="8" t="s">
         <v>5</v>
       </c>
@@ -4893,7 +4893,7 @@
       <c r="G147" s="42"/>
     </row>
     <row r="148" spans="1:7" ht="18">
-      <c r="A148" s="144"/>
+      <c r="A148" s="129"/>
       <c r="B148" s="8" t="s">
         <v>6</v>
       </c>
@@ -4906,7 +4906,7 @@
       <c r="G148" s="42"/>
     </row>
     <row r="149" spans="1:7" ht="18">
-      <c r="A149" s="144"/>
+      <c r="A149" s="129"/>
       <c r="B149" s="8" t="s">
         <v>7</v>
       </c>
@@ -4919,7 +4919,7 @@
       <c r="G149" s="42"/>
     </row>
     <row r="150" spans="1:7" ht="18">
-      <c r="A150" s="144"/>
+      <c r="A150" s="129"/>
       <c r="B150" s="8" t="s">
         <v>8</v>
       </c>
@@ -4930,7 +4930,7 @@
       <c r="G150" s="42"/>
     </row>
     <row r="151" spans="1:7" ht="18">
-      <c r="A151" s="144"/>
+      <c r="A151" s="129"/>
       <c r="B151" s="8" t="s">
         <v>9</v>
       </c>
@@ -4943,7 +4943,7 @@
       <c r="G151" s="42"/>
     </row>
     <row r="152" spans="1:7" ht="19" thickBot="1">
-      <c r="A152" s="145"/>
+      <c r="A152" s="130"/>
       <c r="B152" s="11" t="s">
         <v>10</v>
       </c>
@@ -4956,19 +4956,12 @@
       <c r="G152" s="83"/>
     </row>
     <row r="159" spans="1:7">
-      <c r="C159" s="153" t="s">
+      <c r="C159" s="127" t="s">
         <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A146:A152"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A118:A124"/>
-    <mergeCell ref="A125:A131"/>
-    <mergeCell ref="A132:A138"/>
-    <mergeCell ref="A139:A145"/>
     <mergeCell ref="A97:A103"/>
     <mergeCell ref="A5:A11"/>
     <mergeCell ref="A12:A18"/>
@@ -4983,6 +4976,13 @@
     <mergeCell ref="A41:A47"/>
     <mergeCell ref="A90:A96"/>
     <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A146:A152"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A118:A124"/>
+    <mergeCell ref="A125:A131"/>
+    <mergeCell ref="A132:A138"/>
+    <mergeCell ref="A139:A145"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C159" r:id="rId1" xr:uid="{E53A9555-6A20-3843-B157-6085AF83AF9B}"/>

</xml_diff>